<commit_message>
a man who forgot to commit
</commit_message>
<xml_diff>
--- a/prices.xlsx
+++ b/prices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\juzun\tasks\gas_tank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74771DD1-CEF8-48EB-8944-EC2A85D383A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DAC185-2226-454C-A3A1-7A4ADA136241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{756CE251-4C6A-4012-A30C-462106D57D98}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{756CE251-4C6A-4012-A30C-462106D57D98}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="30" r:id="rId1"/>
@@ -531,21 +531,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C852C912-A669-45F6-9E9C-DFAEECC753F7}">
   <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -560,7 +560,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17">
         <v>45231</v>
       </c>
@@ -575,12 +575,12 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>45261</v>
       </c>
       <c r="B3" s="20">
-        <v>46.631999999999998</v>
+        <v>45.064</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="9"/>
@@ -590,12 +590,12 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>45292</v>
       </c>
       <c r="B4" s="20">
-        <v>48.241999999999997</v>
+        <v>46.421999999999997</v>
       </c>
       <c r="D4" s="21"/>
       <c r="E4" s="9"/>
@@ -605,12 +605,12 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>45323</v>
       </c>
       <c r="B5" s="20">
-        <v>48.790999999999997</v>
+        <v>46.908999999999999</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="4"/>
@@ -620,12 +620,12 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>45352</v>
       </c>
       <c r="B6" s="20">
-        <v>48.317</v>
+        <v>46.515000000000001</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="2"/>
@@ -635,12 +635,12 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>45383</v>
       </c>
       <c r="B7" s="20">
-        <v>47.043999999999997</v>
+        <v>45.639000000000003</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="2"/>
@@ -650,12 +650,12 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>45413</v>
       </c>
       <c r="B8" s="20">
-        <v>46.594000000000001</v>
+        <v>45.335999999999999</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="2"/>
@@ -665,12 +665,12 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>45444</v>
       </c>
       <c r="B9" s="20">
-        <v>46.451999999999998</v>
+        <v>45.276000000000003</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -680,12 +680,12 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>45474</v>
       </c>
       <c r="B10" s="20">
-        <v>46.582000000000001</v>
+        <v>45.423999999999999</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -695,12 +695,12 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>45505</v>
       </c>
       <c r="B11" s="20">
-        <v>46.585999999999999</v>
+        <v>45.511000000000003</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -710,12 +710,12 @@
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>45536</v>
       </c>
       <c r="B12" s="20">
-        <v>46.845999999999997</v>
+        <v>45.753</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="9"/>
@@ -725,12 +725,12 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>45566</v>
       </c>
       <c r="B13" s="20">
-        <v>47.424999999999997</v>
+        <v>46.363</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="9"/>
@@ -740,12 +740,12 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>45597</v>
       </c>
       <c r="B14" s="20">
-        <v>50.1</v>
+        <v>48.993000000000002</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="9"/>
@@ -755,876 +755,876 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>45627</v>
       </c>
       <c r="B15" s="20">
-        <v>51.53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>50.536999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>45658</v>
       </c>
       <c r="B16" s="20">
-        <v>51.62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>50.634</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
         <v>45689</v>
       </c>
       <c r="B17" s="20">
-        <v>51.206000000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>50.234000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>45717</v>
       </c>
       <c r="B18" s="20">
-        <v>49.276000000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>48.353999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>45748</v>
       </c>
       <c r="B19" s="20">
-        <v>43.496000000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>43.451999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>45778</v>
       </c>
       <c r="B20" s="20">
-        <v>41.363999999999997</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>41.307000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>45809</v>
       </c>
       <c r="B21" s="20">
-        <v>40.829000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>40.741999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>45839</v>
       </c>
       <c r="B22" s="20">
-        <v>40.728999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>40.774000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>45870</v>
       </c>
       <c r="B23" s="20">
-        <v>40.959000000000003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>40.999000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <v>45901</v>
       </c>
       <c r="B24" s="20">
-        <v>41.223999999999997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+        <v>41.274000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
         <v>45931</v>
       </c>
       <c r="B25" s="20">
-        <v>41.572000000000003</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>41.51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>45962</v>
       </c>
       <c r="B26" s="20">
-        <v>42.862000000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+        <v>42.850999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>45992</v>
       </c>
       <c r="B27" s="20">
-        <v>43.887</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+        <v>43.889000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>46023</v>
       </c>
       <c r="B28" s="20">
-        <v>44.143999999999998</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+        <v>44.116999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>46054</v>
       </c>
       <c r="B29" s="20">
-        <v>43.543999999999997</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>43.506999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>46082</v>
       </c>
       <c r="B30" s="20">
-        <v>40.993000000000002</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+        <v>40.981999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
         <v>46113</v>
       </c>
       <c r="B31" s="20">
-        <v>37.433999999999997</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+        <v>37.143000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
         <v>46143</v>
       </c>
       <c r="B32" s="20">
-        <v>34.459000000000003</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34.167999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>46174</v>
       </c>
       <c r="B33" s="20">
-        <v>33.734000000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33.442999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>46204</v>
       </c>
       <c r="B34" s="20">
-        <v>33.058999999999997</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+        <v>32.774000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>46235</v>
       </c>
       <c r="B35" s="20">
-        <v>34.094000000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33.798999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>46266</v>
       </c>
       <c r="B36" s="20">
-        <v>34.418999999999997</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34.124000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>46296</v>
       </c>
       <c r="B37" s="20">
-        <v>34.753999999999998</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34.545999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>46327</v>
       </c>
       <c r="B38" s="20">
-        <v>35.643999999999998</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+        <v>35.430999999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>46357</v>
       </c>
       <c r="B39" s="20">
-        <v>36.664000000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36.451000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <v>46388</v>
       </c>
       <c r="B40" s="20">
-        <v>37.014000000000003</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36.783000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
         <v>46419</v>
       </c>
       <c r="B41" s="20">
-        <v>36.658999999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36.442999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>46447</v>
       </c>
       <c r="B42" s="20">
-        <v>34.713000000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34.527999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
         <v>46478</v>
       </c>
       <c r="B43" s="20">
-        <v>29.305</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.308</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>46508</v>
       </c>
       <c r="B44" s="20">
-        <v>28.295000000000002</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+        <v>28.358000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <v>46539</v>
       </c>
       <c r="B45" s="20">
-        <v>28.12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+        <v>28.207999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="17">
         <v>46569</v>
       </c>
       <c r="B46" s="20">
-        <v>27.094999999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+        <v>27.213000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <v>46600</v>
       </c>
       <c r="B47" s="20">
-        <v>27.77</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+        <v>27.933</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>46631</v>
       </c>
       <c r="B48" s="20">
-        <v>28.34</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+        <v>28.558</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
         <v>46661</v>
       </c>
       <c r="B49" s="20">
-        <v>29.071000000000002</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
         <v>46692</v>
       </c>
       <c r="B50" s="20">
-        <v>29.826000000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.882999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>46722</v>
       </c>
       <c r="B51" s="20">
-        <v>30.710999999999999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30.792999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="17">
         <v>46753</v>
       </c>
       <c r="B52" s="20">
-        <v>31.181000000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31.343</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="17">
         <v>46784</v>
       </c>
       <c r="B53" s="20">
-        <v>30.366</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30.523</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
         <v>46813</v>
       </c>
       <c r="B54" s="20">
-        <v>29.731000000000002</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.888000000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="17">
         <v>46844</v>
       </c>
       <c r="B55" s="20">
-        <v>27.018999999999998</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+        <v>27.123999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
         <v>46874</v>
       </c>
       <c r="B56" s="20">
-        <v>26.178999999999998</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+        <v>26.289000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
         <v>46905</v>
       </c>
       <c r="B57" s="20">
-        <v>26.018999999999998</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+        <v>26.129000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="17">
         <v>46935</v>
       </c>
       <c r="B58" s="20">
-        <v>24.619</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+        <v>24.728999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="17">
         <v>46966</v>
       </c>
       <c r="B59" s="20">
-        <v>25.289000000000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+        <v>25.399000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="17">
         <v>46997</v>
       </c>
       <c r="B60" s="20">
-        <v>26.004000000000001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+        <v>26.114000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="17">
         <v>47027</v>
       </c>
       <c r="B61" s="20">
-        <v>28.923999999999999</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.103999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="17">
         <v>47058</v>
       </c>
       <c r="B62" s="20">
-        <v>29.809000000000001</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.994</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="17">
         <v>47088</v>
       </c>
       <c r="B63" s="20">
-        <v>30.594000000000001</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30.779</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="17">
         <v>47119</v>
       </c>
       <c r="B64" s="20">
-        <v>29.376000000000001</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.579000000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="17">
         <v>47150</v>
       </c>
       <c r="B65" s="20">
-        <v>29.17</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.373999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="17">
         <v>47178</v>
       </c>
       <c r="B66" s="20">
-        <v>29.055</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.259</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="17">
         <v>47209</v>
       </c>
       <c r="B67" s="20">
-        <v>28.385000000000002</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+        <v>28.588999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="17">
         <v>47239</v>
       </c>
       <c r="B68" s="20">
-        <v>27.631</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+        <v>27.834</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="17">
         <v>47270</v>
       </c>
       <c r="B69" s="20">
-        <v>26.821000000000002</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+        <v>27.024000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="17">
         <v>47300</v>
       </c>
       <c r="B70" s="20">
-        <v>26.667000000000002</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+        <v>26.869</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="17">
         <v>47331</v>
       </c>
       <c r="B71" s="20">
-        <v>26.904</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+        <v>27.103999999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="17">
         <v>47362</v>
       </c>
       <c r="B72" s="20">
-        <v>27.416</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+        <v>27.614000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="17">
         <v>47392</v>
       </c>
       <c r="B73" s="20">
-        <v>28.238</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+        <v>28.439</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="17">
         <v>47423</v>
       </c>
       <c r="B74" s="20">
-        <v>28.734000000000002</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+        <v>28.934000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="17">
         <v>47453</v>
       </c>
       <c r="B75" s="20">
-        <v>29.145</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.344000000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="17">
         <v>47484</v>
       </c>
       <c r="B76" s="20">
-        <v>29.704000000000001</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.904</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="17">
         <v>47515</v>
       </c>
       <c r="B77" s="20">
-        <v>29.683</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.884</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="17">
         <v>47543</v>
       </c>
       <c r="B78" s="20">
-        <v>29.382000000000001</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.579000000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="17">
         <v>47574</v>
       </c>
       <c r="B79" s="20">
-        <v>29.526</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.724</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="17">
         <v>47604</v>
       </c>
       <c r="B80" s="20">
-        <v>29.15</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.349</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="17">
         <v>47635</v>
       </c>
       <c r="B81" s="20">
-        <v>28.734999999999999</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+        <v>28.934000000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="17">
         <v>47665</v>
       </c>
       <c r="B82" s="20">
-        <v>28.574000000000002</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+        <v>28.774000000000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="17">
         <v>47696</v>
       </c>
       <c r="B83" s="20">
-        <v>28.803999999999998</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.004000000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="17">
         <v>47727</v>
       </c>
       <c r="B84" s="20">
-        <v>29.369</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29.568999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="17">
         <v>47757</v>
       </c>
       <c r="B85" s="20">
-        <v>30.234000000000002</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30.434000000000001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="17">
         <v>47788</v>
       </c>
       <c r="B86" s="20">
-        <v>30.753</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30.954000000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="17">
         <v>47818</v>
       </c>
       <c r="B87" s="20">
-        <v>30.385999999999999</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30.584</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="17">
         <v>47849</v>
       </c>
       <c r="B88" s="20">
-        <v>32.271000000000001</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+        <v>32.469000000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="17">
         <v>47880</v>
       </c>
       <c r="B89" s="20">
-        <v>31.585999999999999</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31.783999999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="17">
         <v>47908</v>
       </c>
       <c r="B90" s="20">
-        <v>31.234999999999999</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31.434000000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="17">
         <v>47939</v>
       </c>
       <c r="B91" s="20">
-        <v>31.645</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31.844000000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="17">
         <v>47969</v>
       </c>
       <c r="B92" s="20">
-        <v>31.25</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31.449000000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="17">
         <v>48000</v>
       </c>
       <c r="B93" s="20">
-        <v>30.83</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31.029</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="17">
         <v>48030</v>
       </c>
       <c r="B94" s="20">
-        <v>30.645</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30.844000000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="17">
         <v>48061</v>
       </c>
       <c r="B95" s="20">
-        <v>30.855</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31.053999999999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="17">
         <v>48092</v>
       </c>
       <c r="B96" s="20">
-        <v>31.375</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31.574000000000002</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="17">
         <v>48122</v>
       </c>
       <c r="B97" s="20">
-        <v>32.195</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+        <v>32.393999999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="17">
         <v>48153</v>
       </c>
       <c r="B98" s="20">
-        <v>32.700000000000003</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+        <v>32.899000000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="17">
         <v>48183</v>
       </c>
       <c r="B99" s="20">
-        <v>32.884999999999998</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33.084000000000003</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="17">
         <v>48214</v>
       </c>
       <c r="B100" s="20">
-        <v>34.854999999999997</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+        <v>35.054000000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="17">
         <v>48245</v>
       </c>
       <c r="B101" s="20">
-        <v>34.159999999999997</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34.359000000000002</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="17">
         <v>48274</v>
       </c>
       <c r="B102" s="20">
-        <v>33.74</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33.939</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="17">
         <v>48305</v>
       </c>
       <c r="B103" s="20">
-        <v>33.715000000000003</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33.914000000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="17">
         <v>48335</v>
       </c>
       <c r="B104" s="20">
-        <v>33.274999999999999</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33.473999999999997</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="17">
         <v>48366</v>
       </c>
       <c r="B105" s="20">
-        <v>32.840000000000003</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33.039000000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="17">
         <v>48396</v>
       </c>
       <c r="B106" s="20">
-        <v>32.64</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+        <v>32.838999999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="17">
         <v>48427</v>
       </c>
       <c r="B107" s="20">
-        <v>32.825000000000003</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33.024000000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="17">
         <v>48458</v>
       </c>
       <c r="B108" s="20">
-        <v>33.31</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33.509</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="17">
         <v>48488</v>
       </c>
       <c r="B109" s="20">
-        <v>34.104999999999997</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34.304000000000002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="17">
         <v>48519</v>
       </c>
       <c r="B110" s="20">
-        <v>34.590000000000003</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34.789000000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="17">
         <v>48549</v>
       </c>
       <c r="B111" s="20">
-        <v>34.814999999999998</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+        <v>35.014000000000003</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="17">
         <v>48580</v>
       </c>
       <c r="B112" s="20">
-        <v>37.625</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+        <v>37.823999999999998</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="17">
         <v>48611</v>
       </c>
       <c r="B113" s="20">
-        <v>37.625</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+        <v>37.823999999999998</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="17">
         <v>48639</v>
       </c>
       <c r="B114" s="20">
-        <v>37.284999999999997</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+        <v>37.484000000000002</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="17">
         <v>48670</v>
       </c>
       <c r="B115" s="20">
-        <v>37.295000000000002</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+        <v>37.494</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="17">
         <v>48700</v>
       </c>
       <c r="B116" s="20">
-        <v>36.895000000000003</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+        <v>37.094000000000001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="17">
         <v>48731</v>
       </c>
       <c r="B117" s="20">
-        <v>36.484999999999999</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36.683999999999997</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="17">
         <v>48761</v>
       </c>
       <c r="B118" s="20">
-        <v>36.305</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36.503999999999998</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="17">
         <v>48792</v>
       </c>
       <c r="B119" s="20">
-        <v>36.505000000000003</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36.704000000000001</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="17">
         <v>48823</v>
       </c>
       <c r="B120" s="20">
-        <v>37.005000000000003</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+        <v>37.204000000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="17">
         <v>48853</v>
       </c>
       <c r="B121" s="20">
-        <v>37.805</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+        <v>38.003999999999998</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="17">
         <v>48884</v>
       </c>
       <c r="B122" s="20">
-        <v>38.305</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+        <v>38.503999999999998</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="17">
         <v>48914</v>
       </c>
       <c r="B123" s="20">
-        <v>38.545000000000002</v>
+        <v>38.744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>